<commit_message>
mise a jour grille eval
</commit_message>
<xml_diff>
--- a/anex/R301_Grille_Evaluation.xlsx
+++ b/anex/R301_Grille_Evaluation.xlsx
@@ -779,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R11" activeCellId="0" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,7 +910,7 @@
         <v>0.5</v>
       </c>
       <c r="D8" s="10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E8" s="10" t="n">
         <v>0.5</v>
@@ -940,7 +940,7 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>0.5</v>
@@ -955,7 +955,7 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>0.5</v>
@@ -970,7 +970,7 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>0.5</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="D13" s="7" t="n">
         <f aca="false">SUM(D8:D12)</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="E13" s="7" t="n">
         <f aca="false">SUM(E8:E12)</f>
@@ -1050,7 +1050,7 @@
         <v>0.5</v>
       </c>
       <c r="D17" s="5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>0.5</v>
@@ -1065,7 +1065,7 @@
         <v>0.5</v>
       </c>
       <c r="D18" s="5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>0.5</v>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="D20" s="15" t="n">
         <f aca="false">SUM(D14:D19)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="15" t="n">
         <f aca="false">SUM(E14:E19)</f>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D26" s="17" t="n">
         <f aca="false">SUM(D7,D13,D20,D25)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E26" s="17" t="n">
         <f aca="false">SUM(E7,E13,E20,E25)</f>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="D47" s="26" t="n">
         <f aca="false">ROUND(D26*(D28+D45)*4,0)/4</f>
-        <v>7.5</v>
+        <v>12</v>
       </c>
       <c r="E47" s="26" t="n">
         <f aca="false">ROUND(E26*(E28+E45)*4,0)/4</f>

</xml_diff>